<commit_message>
final housekeeping - making sure the py generation scripts work as expected
</commit_message>
<xml_diff>
--- a/dbt_code_generation_workflow/ip/data_src_a_data_dictionary.xlsx
+++ b/dbt_code_generation_workflow/ip/data_src_a_data_dictionary.xlsx
@@ -8,15 +8,15 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/paulfry/Dropbox/tech/code/git-repos/dbt_repos/dbt/dbt_code_generation_workflow/ip/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{791BEF27-2B7F-B242-87FC-2AED1EE12323}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C1C58A70-EF49-D34E-A513-6C5A0FA73FA6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-31140" yWindow="2480" windowWidth="28800" windowHeight="17500" xr2:uid="{F5447BD4-51BA-CB4A-AA03-46A64813458D}"/>
+    <workbookView xWindow="-31140" yWindow="2480" windowWidth="28800" windowHeight="17500" activeTab="1" xr2:uid="{F5447BD4-51BA-CB4A-AA03-46A64813458D}"/>
   </bookViews>
   <sheets>
     <sheet name="table_a" sheetId="1" r:id="rId1"/>
     <sheet name="table_b" sheetId="2" r:id="rId2"/>
   </sheets>
-  <calcPr calcId="181029" iterateDelta="1E-4"/>
+  <calcPr calcId="181029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -549,8 +549,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{21A3F06E-3DE3-9748-8162-6D49E20586D1}">
   <dimension ref="B2:N7"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="M3" sqref="M3"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="H3" sqref="H3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -729,7 +729,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{89E301CF-5EFF-2C41-B661-9A4150B69AC2}">
   <dimension ref="B2:N6"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="M3" sqref="M3"/>
     </sheetView>
   </sheetViews>

</xml_diff>